<commit_message>
Update Project Structure based on recommendations from https://medium.com/bcggamma/data-science-python-best-practices-fdb16fdedf82
Added package structure, configuration management, logging
</commit_message>
<xml_diff>
--- a/Electronics/Balance Bot Electrical Connection.xlsx
+++ b/Electronics/Balance Bot Electrical Connection.xlsx
@@ -16,6 +16,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Matrix!$A$1:$DO$56</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -6391,7 +6392,7 @@
   <dimension ref="A1:DO126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
@@ -22648,11 +22649,11 @@
         <v>42</v>
       </c>
       <c r="B24" s="91">
-        <f t="shared" ref="B24:B27" si="0">0.127*92^((36-A24)/39)</f>
+        <f t="shared" ref="B24:B31" si="0">0.127*92^((36-A24)/39)</f>
         <v>6.3340650141794921E-2</v>
       </c>
       <c r="C24" s="93">
-        <f t="shared" ref="C24:C27" si="1">PI()*(B24/2)^2</f>
+        <f t="shared" ref="C24:C31" si="1">PI()*(B24/2)^2</f>
         <v>3.1510472455674311E-3</v>
       </c>
     </row>
@@ -22712,11 +22713,11 @@
         <v>34</v>
       </c>
       <c r="B28" s="91">
-        <f t="shared" ref="B28:B30" si="2">0.127*92^((36-A28)/39)</f>
+        <f t="shared" si="0"/>
         <v>0.16014404318711942</v>
       </c>
       <c r="C28" s="93">
-        <f t="shared" ref="C28:C30" si="3">PI()*(B28/2)^2</f>
+        <f t="shared" si="1"/>
         <v>2.0142411280237475E-2</v>
       </c>
     </row>
@@ -22725,11 +22726,11 @@
         <v>32</v>
       </c>
       <c r="B29" s="91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.20193790998675565</v>
       </c>
       <c r="C29" s="93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3.2027688472636276E-2</v>
       </c>
     </row>
@@ -22738,11 +22739,11 @@
         <v>30</v>
       </c>
       <c r="B30" s="91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.25463900297665848</v>
       </c>
       <c r="C30" s="93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.0926019463551769E-2</v>
       </c>
     </row>
@@ -22751,11 +22752,11 @@
         <v>28</v>
       </c>
       <c r="B31" s="91">
-        <f>0.127*92^((36-A31)/39)</f>
+        <f t="shared" si="0"/>
         <v>0.32109385425054349</v>
       </c>
       <c r="C31" s="93">
-        <f>PI()*(B31/2)^2</f>
+        <f t="shared" si="1"/>
         <v>8.0975542790665211E-2</v>
       </c>
       <c r="J31" s="1">
@@ -22768,11 +22769,11 @@
         <v>26</v>
       </c>
       <c r="B32" s="91">
-        <f t="shared" ref="B32:B39" si="4">0.127*92^((36-A32)/39)</f>
+        <f t="shared" ref="B32:B39" si="2">0.127*92^((36-A32)/39)</f>
         <v>0.40489187450565089</v>
       </c>
       <c r="C32" s="93">
-        <f t="shared" ref="C32:C39" si="5">PI()*(B32/2)^2</f>
+        <f t="shared" ref="C32:C39" si="3">PI()*(B32/2)^2</f>
         <v>0.12875615646606325</v>
       </c>
     </row>
@@ -22781,11 +22782,11 @@
         <v>24</v>
       </c>
       <c r="B33" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.5105592270625724</v>
       </c>
       <c r="C33" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.20473030814712212</v>
       </c>
     </row>
@@ -22794,11 +22795,11 @@
         <v>22</v>
       </c>
       <c r="B34" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.64380329849047946</v>
       </c>
       <c r="C34" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.32553394124546686</v>
       </c>
     </row>
@@ -22807,11 +22808,11 @@
         <v>20</v>
       </c>
       <c r="B35" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.81182097037377388</v>
       </c>
       <c r="C35" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.51761924192803854</v>
       </c>
     </row>
@@ -22820,11 +22821,11 @@
         <v>18</v>
       </c>
       <c r="B36" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.0236873428326523</v>
       </c>
       <c r="C36" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.8230468337313146</v>
       </c>
     </row>
@@ -22833,11 +22834,11 @@
         <v>16</v>
       </c>
       <c r="B37" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2908459058322816</v>
       </c>
       <c r="C37" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.3086957277552631</v>
       </c>
     </row>
@@ -22846,11 +22847,11 @@
         <v>14</v>
       </c>
       <c r="B38" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.6277266337915051</v>
       </c>
       <c r="C38" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.080907717098377</v>
       </c>
     </row>
@@ -22859,11 +22860,11 @@
         <v>12</v>
       </c>
       <c r="B39" s="91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2.0525253884939478</v>
       </c>
       <c r="C39" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3.308772876111477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor update to get Pi and Computer synced
</commit_message>
<xml_diff>
--- a/Electronics/Balance Bot Electrical Connection.xlsx
+++ b/Electronics/Balance Bot Electrical Connection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3660" windowWidth="15720" windowHeight="7220"/>
+    <workbookView xWindow="2378" yWindow="3660" windowWidth="15720" windowHeight="7223"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Matrix!$A$1:$DO$56</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2197,6 +2196,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2215,37 +2232,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6392,50 +6391,50 @@
   <dimension ref="A1:DO126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="8" topLeftCell="X9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.05859375" defaultRowHeight="13.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.64453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.703125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="6.76171875" style="1" customWidth="1"/>
-    <col min="6" max="25" width="7.9375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9.234375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.41015625" style="1" customWidth="1"/>
-    <col min="28" max="29" width="8.64453125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="9.234375" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.41015625" style="1" customWidth="1"/>
-    <col min="32" max="33" width="8.64453125" style="1" customWidth="1"/>
-    <col min="34" max="51" width="9.1171875" style="1" customWidth="1"/>
-    <col min="52" max="59" width="11.64453125" style="1" customWidth="1"/>
-    <col min="60" max="61" width="9.1171875" style="1" customWidth="1"/>
-    <col min="62" max="62" width="11.05859375" style="1" customWidth="1"/>
-    <col min="63" max="65" width="10.87890625" style="1" customWidth="1"/>
-    <col min="66" max="67" width="11.9375" style="1" customWidth="1"/>
-    <col min="68" max="69" width="13.05859375" style="1" customWidth="1"/>
-    <col min="70" max="70" width="9.1171875" style="1" customWidth="1"/>
-    <col min="71" max="71" width="10.76171875" style="1" customWidth="1"/>
-    <col min="72" max="72" width="9.1171875" style="1" customWidth="1"/>
-    <col min="73" max="73" width="10.76171875" style="1" customWidth="1"/>
-    <col min="74" max="82" width="9.1171875" style="1" customWidth="1"/>
-    <col min="83" max="83" width="10.76171875" style="1" customWidth="1"/>
-    <col min="84" max="84" width="9.1171875" style="1" customWidth="1"/>
-    <col min="85" max="85" width="10.76171875" style="1" customWidth="1"/>
-    <col min="86" max="119" width="9.1171875" style="1" customWidth="1"/>
-    <col min="120" max="16384" width="9.05859375" style="1"/>
+    <col min="1" max="1" width="50.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.73046875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="6.73046875" style="1" customWidth="1"/>
+    <col min="6" max="25" width="7.9296875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.19921875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="9.3984375" style="1" customWidth="1"/>
+    <col min="28" max="29" width="8.6640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="9.19921875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.3984375" style="1" customWidth="1"/>
+    <col min="32" max="33" width="8.6640625" style="1" customWidth="1"/>
+    <col min="34" max="51" width="9.1328125" style="1" customWidth="1"/>
+    <col min="52" max="59" width="11.6640625" style="1" customWidth="1"/>
+    <col min="60" max="61" width="9.1328125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="11.06640625" style="1" customWidth="1"/>
+    <col min="63" max="65" width="10.86328125" style="1" customWidth="1"/>
+    <col min="66" max="67" width="11.9296875" style="1" customWidth="1"/>
+    <col min="68" max="69" width="13.06640625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="9.1328125" style="1" customWidth="1"/>
+    <col min="71" max="71" width="10.73046875" style="1" customWidth="1"/>
+    <col min="72" max="72" width="9.1328125" style="1" customWidth="1"/>
+    <col min="73" max="73" width="10.73046875" style="1" customWidth="1"/>
+    <col min="74" max="82" width="9.1328125" style="1" customWidth="1"/>
+    <col min="83" max="83" width="10.73046875" style="1" customWidth="1"/>
+    <col min="84" max="84" width="9.1328125" style="1" customWidth="1"/>
+    <col min="85" max="85" width="10.73046875" style="1" customWidth="1"/>
+    <col min="86" max="119" width="9.1328125" style="1" customWidth="1"/>
+    <col min="120" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" ht="18" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:119" ht="18" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:119" x14ac:dyDescent="0.35">
       <c r="BD2" s="135" t="s">
         <v>258</v>
       </c>
@@ -6449,8 +6448,8 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:119" ht="14" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:119" ht="42.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:119" ht="13.9" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:119" ht="42.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="126" t="s">
         <v>216</v>
       </c>
@@ -6460,162 +6459,162 @@
       <c r="C4" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="157" t="s">
+      <c r="D4" s="151" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="159"/>
-      <c r="F4" s="154" t="s">
+      <c r="E4" s="153"/>
+      <c r="F4" s="160" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="155"/>
-      <c r="M4" s="155"/>
-      <c r="N4" s="155"/>
-      <c r="O4" s="155"/>
-      <c r="P4" s="155"/>
-      <c r="Q4" s="155"/>
-      <c r="R4" s="155"/>
-      <c r="S4" s="155"/>
-      <c r="T4" s="155"/>
-      <c r="U4" s="155"/>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
-      <c r="Z4" s="151" t="s">
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
+      <c r="L4" s="161"/>
+      <c r="M4" s="161"/>
+      <c r="N4" s="161"/>
+      <c r="O4" s="161"/>
+      <c r="P4" s="161"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="161"/>
+      <c r="S4" s="161"/>
+      <c r="T4" s="161"/>
+      <c r="U4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
+      <c r="Z4" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="AA4" s="152"/>
-      <c r="AB4" s="152"/>
-      <c r="AC4" s="153"/>
-      <c r="AD4" s="151" t="s">
+      <c r="AA4" s="158"/>
+      <c r="AB4" s="158"/>
+      <c r="AC4" s="159"/>
+      <c r="AD4" s="157" t="s">
         <v>151</v>
       </c>
-      <c r="AE4" s="152"/>
-      <c r="AF4" s="152"/>
-      <c r="AG4" s="153"/>
-      <c r="AH4" s="157" t="s">
+      <c r="AE4" s="158"/>
+      <c r="AF4" s="158"/>
+      <c r="AG4" s="159"/>
+      <c r="AH4" s="151" t="s">
         <v>152</v>
       </c>
-      <c r="AI4" s="158"/>
-      <c r="AJ4" s="158"/>
-      <c r="AK4" s="158"/>
-      <c r="AL4" s="158"/>
-      <c r="AM4" s="160"/>
-      <c r="AN4" s="161" t="s">
+      <c r="AI4" s="152"/>
+      <c r="AJ4" s="152"/>
+      <c r="AK4" s="152"/>
+      <c r="AL4" s="152"/>
+      <c r="AM4" s="155"/>
+      <c r="AN4" s="156" t="s">
         <v>153</v>
       </c>
-      <c r="AO4" s="158"/>
-      <c r="AP4" s="158"/>
-      <c r="AQ4" s="158"/>
-      <c r="AR4" s="158"/>
-      <c r="AS4" s="158"/>
-      <c r="AT4" s="158"/>
-      <c r="AU4" s="158"/>
-      <c r="AV4" s="158"/>
-      <c r="AW4" s="159"/>
-      <c r="AX4" s="157" t="s">
+      <c r="AO4" s="152"/>
+      <c r="AP4" s="152"/>
+      <c r="AQ4" s="152"/>
+      <c r="AR4" s="152"/>
+      <c r="AS4" s="152"/>
+      <c r="AT4" s="152"/>
+      <c r="AU4" s="152"/>
+      <c r="AV4" s="152"/>
+      <c r="AW4" s="153"/>
+      <c r="AX4" s="151" t="s">
         <v>154</v>
       </c>
-      <c r="AY4" s="158"/>
-      <c r="AZ4" s="158"/>
-      <c r="BA4" s="158"/>
-      <c r="BB4" s="158"/>
-      <c r="BC4" s="158"/>
-      <c r="BD4" s="158"/>
-      <c r="BE4" s="158"/>
-      <c r="BF4" s="158"/>
-      <c r="BG4" s="159"/>
-      <c r="BH4" s="157" t="s">
+      <c r="AY4" s="152"/>
+      <c r="AZ4" s="152"/>
+      <c r="BA4" s="152"/>
+      <c r="BB4" s="152"/>
+      <c r="BC4" s="152"/>
+      <c r="BD4" s="152"/>
+      <c r="BE4" s="152"/>
+      <c r="BF4" s="152"/>
+      <c r="BG4" s="153"/>
+      <c r="BH4" s="151" t="s">
         <v>155</v>
       </c>
-      <c r="BI4" s="158"/>
-      <c r="BJ4" s="158"/>
-      <c r="BK4" s="158"/>
-      <c r="BL4" s="158"/>
-      <c r="BM4" s="158"/>
-      <c r="BN4" s="158"/>
-      <c r="BO4" s="158"/>
-      <c r="BP4" s="158"/>
-      <c r="BQ4" s="159"/>
-      <c r="BR4" s="157" t="s">
+      <c r="BI4" s="152"/>
+      <c r="BJ4" s="152"/>
+      <c r="BK4" s="152"/>
+      <c r="BL4" s="152"/>
+      <c r="BM4" s="152"/>
+      <c r="BN4" s="152"/>
+      <c r="BO4" s="152"/>
+      <c r="BP4" s="152"/>
+      <c r="BQ4" s="153"/>
+      <c r="BR4" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="BS4" s="160"/>
-      <c r="BT4" s="161" t="s">
+      <c r="BS4" s="155"/>
+      <c r="BT4" s="156" t="s">
         <v>157</v>
       </c>
-      <c r="BU4" s="159"/>
-      <c r="BV4" s="157" t="s">
+      <c r="BU4" s="153"/>
+      <c r="BV4" s="151" t="s">
         <v>160</v>
       </c>
-      <c r="BW4" s="158"/>
-      <c r="BX4" s="158"/>
-      <c r="BY4" s="159"/>
-      <c r="BZ4" s="162" t="s">
+      <c r="BW4" s="152"/>
+      <c r="BX4" s="152"/>
+      <c r="BY4" s="153"/>
+      <c r="BZ4" s="154" t="s">
         <v>233</v>
       </c>
-      <c r="CA4" s="158"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="159"/>
-      <c r="CD4" s="157" t="s">
+      <c r="CA4" s="152"/>
+      <c r="CB4" s="152"/>
+      <c r="CC4" s="153"/>
+      <c r="CD4" s="151" t="s">
         <v>158</v>
       </c>
-      <c r="CE4" s="160"/>
-      <c r="CF4" s="161" t="s">
+      <c r="CE4" s="155"/>
+      <c r="CF4" s="156" t="s">
         <v>159</v>
       </c>
-      <c r="CG4" s="159"/>
-      <c r="CH4" s="157" t="s">
+      <c r="CG4" s="153"/>
+      <c r="CH4" s="151" t="s">
         <v>162</v>
       </c>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="158"/>
-      <c r="CK4" s="159"/>
-      <c r="CL4" s="162" t="s">
+      <c r="CI4" s="152"/>
+      <c r="CJ4" s="152"/>
+      <c r="CK4" s="153"/>
+      <c r="CL4" s="154" t="s">
         <v>275</v>
       </c>
-      <c r="CM4" s="158"/>
-      <c r="CN4" s="158"/>
-      <c r="CO4" s="159"/>
-      <c r="CP4" s="157" t="s">
+      <c r="CM4" s="152"/>
+      <c r="CN4" s="152"/>
+      <c r="CO4" s="153"/>
+      <c r="CP4" s="151" t="s">
         <v>164</v>
       </c>
-      <c r="CQ4" s="158"/>
-      <c r="CR4" s="158"/>
-      <c r="CS4" s="158"/>
-      <c r="CT4" s="158"/>
-      <c r="CU4" s="158"/>
-      <c r="CV4" s="158"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="158"/>
-      <c r="CY4" s="159"/>
-      <c r="CZ4" s="157" t="s">
+      <c r="CQ4" s="152"/>
+      <c r="CR4" s="152"/>
+      <c r="CS4" s="152"/>
+      <c r="CT4" s="152"/>
+      <c r="CU4" s="152"/>
+      <c r="CV4" s="152"/>
+      <c r="CW4" s="152"/>
+      <c r="CX4" s="152"/>
+      <c r="CY4" s="153"/>
+      <c r="CZ4" s="151" t="s">
         <v>165</v>
       </c>
-      <c r="DA4" s="158"/>
-      <c r="DB4" s="158"/>
-      <c r="DC4" s="158"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="158"/>
-      <c r="DF4" s="158"/>
-      <c r="DG4" s="159"/>
-      <c r="DH4" s="157" t="s">
+      <c r="DA4" s="152"/>
+      <c r="DB4" s="152"/>
+      <c r="DC4" s="152"/>
+      <c r="DD4" s="152"/>
+      <c r="DE4" s="152"/>
+      <c r="DF4" s="152"/>
+      <c r="DG4" s="153"/>
+      <c r="DH4" s="151" t="s">
         <v>178</v>
       </c>
-      <c r="DI4" s="158"/>
-      <c r="DJ4" s="158"/>
-      <c r="DK4" s="158"/>
-      <c r="DL4" s="158"/>
-      <c r="DM4" s="158"/>
-      <c r="DN4" s="158"/>
-      <c r="DO4" s="159"/>
+      <c r="DI4" s="152"/>
+      <c r="DJ4" s="152"/>
+      <c r="DK4" s="152"/>
+      <c r="DL4" s="152"/>
+      <c r="DM4" s="152"/>
+      <c r="DN4" s="152"/>
+      <c r="DO4" s="153"/>
     </row>
-    <row r="5" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A5" s="127" t="s">
         <v>217</v>
       </c>
@@ -6974,7 +6973,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:119" ht="27.35" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:119" ht="27" x14ac:dyDescent="0.35">
       <c r="A6" s="127" t="s">
         <v>218</v>
       </c>
@@ -7333,7 +7332,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:119" ht="27.35" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:119" ht="27" x14ac:dyDescent="0.35">
       <c r="A7" s="127" t="s">
         <v>228</v>
       </c>
@@ -7668,7 +7667,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:119" ht="62.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:119" ht="62.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="141" t="s">
         <v>284</v>
       </c>
@@ -8027,7 +8026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A9" s="147" t="s">
         <v>212</v>
       </c>
@@ -8152,7 +8151,7 @@
       <c r="DN9" s="116"/>
       <c r="DO9" s="116"/>
     </row>
-    <row r="10" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A10" s="148" t="s">
         <v>213</v>
       </c>
@@ -8277,7 +8276,7 @@
       <c r="DN10" s="116"/>
       <c r="DO10" s="116"/>
     </row>
-    <row r="11" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A11" s="148" t="s">
         <v>290</v>
       </c>
@@ -8402,7 +8401,7 @@
       <c r="DN11" s="116"/>
       <c r="DO11" s="116"/>
     </row>
-    <row r="12" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A12" s="128" t="s">
         <v>214</v>
       </c>
@@ -8527,7 +8526,7 @@
       <c r="DN12" s="116"/>
       <c r="DO12" s="116"/>
     </row>
-    <row r="13" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A13" s="128" t="s">
         <v>219</v>
       </c>
@@ -8652,7 +8651,7 @@
       <c r="DN13" s="116"/>
       <c r="DO13" s="116"/>
     </row>
-    <row r="14" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A14" s="128" t="s">
         <v>220</v>
       </c>
@@ -8777,7 +8776,7 @@
       <c r="DN14" s="116"/>
       <c r="DO14" s="116"/>
     </row>
-    <row r="15" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A15" s="118" t="s">
         <v>221</v>
       </c>
@@ -8902,7 +8901,7 @@
       <c r="DN15" s="116"/>
       <c r="DO15" s="116"/>
     </row>
-    <row r="16" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A16" s="123" t="s">
         <v>234</v>
       </c>
@@ -9027,7 +9026,7 @@
       <c r="DN16" s="116"/>
       <c r="DO16" s="116"/>
     </row>
-    <row r="17" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A17" s="130" t="s">
         <v>238</v>
       </c>
@@ -9152,7 +9151,7 @@
       <c r="DN17" s="116"/>
       <c r="DO17" s="116"/>
     </row>
-    <row r="18" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A18" s="149" t="s">
         <v>240</v>
       </c>
@@ -9277,7 +9276,7 @@
       <c r="DN18" s="116"/>
       <c r="DO18" s="116"/>
     </row>
-    <row r="19" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A19" s="150" t="s">
         <v>239</v>
       </c>
@@ -9402,7 +9401,7 @@
       <c r="DN19" s="116"/>
       <c r="DO19" s="116"/>
     </row>
-    <row r="20" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A20" s="150" t="s">
         <v>243</v>
       </c>
@@ -9527,7 +9526,7 @@
       <c r="DN20" s="116"/>
       <c r="DO20" s="116"/>
     </row>
-    <row r="21" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A21" s="123" t="s">
         <v>245</v>
       </c>
@@ -9652,7 +9651,7 @@
       <c r="DN21" s="116"/>
       <c r="DO21" s="116"/>
     </row>
-    <row r="22" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A22" s="150" t="s">
         <v>246</v>
       </c>
@@ -9777,7 +9776,7 @@
       <c r="DN22" s="116"/>
       <c r="DO22" s="116"/>
     </row>
-    <row r="23" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A23" s="150" t="s">
         <v>247</v>
       </c>
@@ -9902,7 +9901,7 @@
       <c r="DN23" s="116"/>
       <c r="DO23" s="116"/>
     </row>
-    <row r="24" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A24" s="118" t="s">
         <v>222</v>
       </c>
@@ -10027,7 +10026,7 @@
       <c r="DN24" s="116"/>
       <c r="DO24" s="116"/>
     </row>
-    <row r="25" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A25" s="118" t="s">
         <v>223</v>
       </c>
@@ -10152,7 +10151,7 @@
       <c r="DN25" s="116"/>
       <c r="DO25" s="116"/>
     </row>
-    <row r="26" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A26" s="150" t="s">
         <v>248</v>
       </c>
@@ -10277,7 +10276,7 @@
       <c r="DN26" s="116"/>
       <c r="DO26" s="116"/>
     </row>
-    <row r="27" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A27" s="150" t="s">
         <v>249</v>
       </c>
@@ -10402,7 +10401,7 @@
       <c r="DN27" s="116"/>
       <c r="DO27" s="116"/>
     </row>
-    <row r="28" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A28" s="123" t="s">
         <v>229</v>
       </c>
@@ -10527,7 +10526,7 @@
       <c r="DN28" s="116"/>
       <c r="DO28" s="116"/>
     </row>
-    <row r="29" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A29" s="123" t="s">
         <v>230</v>
       </c>
@@ -10652,7 +10651,7 @@
       <c r="DN29" s="116"/>
       <c r="DO29" s="116"/>
     </row>
-    <row r="30" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A30" s="130" t="s">
         <v>266</v>
       </c>
@@ -10777,7 +10776,7 @@
       <c r="DN30" s="116"/>
       <c r="DO30" s="116"/>
     </row>
-    <row r="31" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A31" s="130" t="s">
         <v>267</v>
       </c>
@@ -10902,7 +10901,7 @@
       <c r="DN31" s="116"/>
       <c r="DO31" s="116"/>
     </row>
-    <row r="32" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A32" s="130" t="s">
         <v>276</v>
       </c>
@@ -11027,7 +11026,7 @@
       <c r="DN32" s="116"/>
       <c r="DO32" s="116"/>
     </row>
-    <row r="33" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A33" s="130" t="s">
         <v>277</v>
       </c>
@@ -11152,7 +11151,7 @@
       <c r="DN33" s="116"/>
       <c r="DO33" s="116"/>
     </row>
-    <row r="34" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A34" s="118" t="s">
         <v>280</v>
       </c>
@@ -11277,7 +11276,7 @@
       <c r="DN34" s="116"/>
       <c r="DO34" s="116"/>
     </row>
-    <row r="35" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A35" s="118" t="s">
         <v>281</v>
       </c>
@@ -11402,7 +11401,7 @@
       <c r="DN35" s="116"/>
       <c r="DO35" s="116"/>
     </row>
-    <row r="36" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A36" s="118" t="s">
         <v>282</v>
       </c>
@@ -11527,7 +11526,7 @@
       <c r="DN36" s="116"/>
       <c r="DO36" s="116"/>
     </row>
-    <row r="37" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A37" s="130" t="s">
         <v>278</v>
       </c>
@@ -11652,7 +11651,7 @@
       <c r="DN37" s="116"/>
       <c r="DO37" s="116"/>
     </row>
-    <row r="38" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A38" s="123" t="s">
         <v>279</v>
       </c>
@@ -11777,7 +11776,7 @@
       <c r="DN38" s="116"/>
       <c r="DO38" s="116"/>
     </row>
-    <row r="39" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A39" s="118" t="s">
         <v>224</v>
       </c>
@@ -11902,7 +11901,7 @@
       <c r="DN39" s="116"/>
       <c r="DO39" s="116"/>
     </row>
-    <row r="40" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A40" s="118" t="s">
         <v>225</v>
       </c>
@@ -12027,7 +12026,7 @@
       <c r="DN40" s="116"/>
       <c r="DO40" s="116"/>
     </row>
-    <row r="41" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A41" s="118" t="s">
         <v>226</v>
       </c>
@@ -12152,7 +12151,7 @@
       <c r="DN41" s="116"/>
       <c r="DO41" s="116"/>
     </row>
-    <row r="42" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A42" s="118" t="s">
         <v>227</v>
       </c>
@@ -12277,7 +12276,7 @@
       <c r="DN42" s="116"/>
       <c r="DO42" s="116"/>
     </row>
-    <row r="43" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A43" s="123" t="s">
         <v>235</v>
       </c>
@@ -12402,7 +12401,7 @@
       <c r="DN43" s="116"/>
       <c r="DO43" s="116"/>
     </row>
-    <row r="44" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A44" s="130" t="s">
         <v>241</v>
       </c>
@@ -12527,7 +12526,7 @@
       <c r="DN44" s="116"/>
       <c r="DO44" s="116"/>
     </row>
-    <row r="45" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A45" s="123" t="s">
         <v>242</v>
       </c>
@@ -12652,7 +12651,7 @@
       <c r="DN45" s="116"/>
       <c r="DO45" s="116"/>
     </row>
-    <row r="46" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A46" s="123" t="s">
         <v>244</v>
       </c>
@@ -12777,7 +12776,7 @@
       <c r="DN46" s="116"/>
       <c r="DO46" s="116"/>
     </row>
-    <row r="47" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A47" s="123" t="s">
         <v>286</v>
       </c>
@@ -12902,7 +12901,7 @@
       <c r="DN47" s="116"/>
       <c r="DO47" s="116"/>
     </row>
-    <row r="48" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A48" s="123" t="s">
         <v>262</v>
       </c>
@@ -13027,7 +13026,7 @@
       <c r="DN48" s="116"/>
       <c r="DO48" s="116"/>
     </row>
-    <row r="49" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A49" s="123" t="s">
         <v>263</v>
       </c>
@@ -13152,7 +13151,7 @@
       <c r="DN49" s="116"/>
       <c r="DO49" s="116"/>
     </row>
-    <row r="50" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A50" s="123" t="s">
         <v>264</v>
       </c>
@@ -13277,7 +13276,7 @@
       <c r="DN50" s="116"/>
       <c r="DO50" s="116"/>
     </row>
-    <row r="51" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A51" s="123" t="s">
         <v>265</v>
       </c>
@@ -13402,7 +13401,7 @@
       <c r="DN51" s="116"/>
       <c r="DO51" s="116"/>
     </row>
-    <row r="52" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A52" s="123" t="s">
         <v>232</v>
       </c>
@@ -13527,7 +13526,7 @@
       <c r="DN52" s="116"/>
       <c r="DO52" s="116"/>
     </row>
-    <row r="53" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A53" s="123" t="s">
         <v>231</v>
       </c>
@@ -13652,7 +13651,7 @@
       <c r="DN53" s="116"/>
       <c r="DO53" s="116"/>
     </row>
-    <row r="54" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A54" s="130" t="s">
         <v>236</v>
       </c>
@@ -13777,7 +13776,7 @@
       <c r="DN54" s="116"/>
       <c r="DO54" s="116"/>
     </row>
-    <row r="55" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A55" s="130" t="s">
         <v>237</v>
       </c>
@@ -13902,7 +13901,7 @@
       <c r="DN55" s="116"/>
       <c r="DO55" s="116"/>
     </row>
-    <row r="56" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A56" s="123" t="s">
         <v>285</v>
       </c>
@@ -14027,7 +14026,7 @@
       <c r="DN56" s="116"/>
       <c r="DO56" s="116"/>
     </row>
-    <row r="57" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A57" s="129"/>
       <c r="B57" s="117"/>
       <c r="C57" s="116"/>
@@ -14148,7 +14147,7 @@
       <c r="DN57" s="116"/>
       <c r="DO57" s="116"/>
     </row>
-    <row r="58" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A58" s="129"/>
       <c r="B58" s="115"/>
       <c r="C58" s="116"/>
@@ -14269,7 +14268,7 @@
       <c r="DN58" s="116"/>
       <c r="DO58" s="116"/>
     </row>
-    <row r="59" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A59" s="129"/>
       <c r="B59" s="117"/>
       <c r="C59" s="116"/>
@@ -14390,7 +14389,7 @@
       <c r="DN59" s="116"/>
       <c r="DO59" s="116"/>
     </row>
-    <row r="60" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A60" s="129"/>
       <c r="B60" s="117"/>
       <c r="C60" s="116"/>
@@ -14511,7 +14510,7 @@
       <c r="DN60" s="116"/>
       <c r="DO60" s="116"/>
     </row>
-    <row r="61" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A61" s="129"/>
       <c r="B61" s="117"/>
       <c r="C61" s="116"/>
@@ -14632,7 +14631,7 @@
       <c r="DN61" s="116"/>
       <c r="DO61" s="116"/>
     </row>
-    <row r="62" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A62" s="129"/>
       <c r="B62" s="117"/>
       <c r="C62" s="116"/>
@@ -14753,7 +14752,7 @@
       <c r="DN62" s="116"/>
       <c r="DO62" s="116"/>
     </row>
-    <row r="63" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A63" s="129"/>
       <c r="B63" s="117"/>
       <c r="C63" s="116"/>
@@ -14874,7 +14873,7 @@
       <c r="DN63" s="116"/>
       <c r="DO63" s="116"/>
     </row>
-    <row r="64" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A64" s="129"/>
       <c r="B64" s="117"/>
       <c r="C64" s="116"/>
@@ -14995,7 +14994,7 @@
       <c r="DN64" s="116"/>
       <c r="DO64" s="116"/>
     </row>
-    <row r="65" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A65" s="129"/>
       <c r="B65" s="117"/>
       <c r="C65" s="116"/>
@@ -15116,7 +15115,7 @@
       <c r="DN65" s="116"/>
       <c r="DO65" s="116"/>
     </row>
-    <row r="66" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A66" s="129"/>
       <c r="B66" s="117"/>
       <c r="C66" s="116"/>
@@ -15237,7 +15236,7 @@
       <c r="DN66" s="116"/>
       <c r="DO66" s="116"/>
     </row>
-    <row r="67" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A67" s="129"/>
       <c r="B67" s="117"/>
       <c r="C67" s="116"/>
@@ -15358,7 +15357,7 @@
       <c r="DN67" s="116"/>
       <c r="DO67" s="116"/>
     </row>
-    <row r="68" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A68" s="129"/>
       <c r="B68" s="115"/>
       <c r="C68" s="116"/>
@@ -15479,7 +15478,7 @@
       <c r="DN68" s="116"/>
       <c r="DO68" s="116"/>
     </row>
-    <row r="69" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A69" s="129"/>
       <c r="B69" s="117"/>
       <c r="C69" s="116"/>
@@ -15600,7 +15599,7 @@
       <c r="DN69" s="116"/>
       <c r="DO69" s="116"/>
     </row>
-    <row r="70" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A70" s="129"/>
       <c r="B70" s="117"/>
       <c r="C70" s="116"/>
@@ -15721,7 +15720,7 @@
       <c r="DN70" s="116"/>
       <c r="DO70" s="116"/>
     </row>
-    <row r="71" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A71" s="129"/>
       <c r="B71" s="117"/>
       <c r="C71" s="116"/>
@@ -15842,7 +15841,7 @@
       <c r="DN71" s="116"/>
       <c r="DO71" s="116"/>
     </row>
-    <row r="72" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A72" s="129"/>
       <c r="B72" s="117"/>
       <c r="C72" s="116"/>
@@ -15963,7 +15962,7 @@
       <c r="DN72" s="116"/>
       <c r="DO72" s="116"/>
     </row>
-    <row r="73" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A73" s="115"/>
       <c r="B73" s="117"/>
       <c r="C73" s="116"/>
@@ -16084,7 +16083,7 @@
       <c r="DN73" s="116"/>
       <c r="DO73" s="116"/>
     </row>
-    <row r="74" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A74" s="115"/>
       <c r="B74" s="117"/>
       <c r="C74" s="116"/>
@@ -16205,7 +16204,7 @@
       <c r="DN74" s="116"/>
       <c r="DO74" s="116"/>
     </row>
-    <row r="75" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A75" s="115"/>
       <c r="B75" s="117"/>
       <c r="C75" s="116"/>
@@ -16326,7 +16325,7 @@
       <c r="DN75" s="116"/>
       <c r="DO75" s="116"/>
     </row>
-    <row r="76" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A76" s="115"/>
       <c r="B76" s="117"/>
       <c r="C76" s="116"/>
@@ -16447,7 +16446,7 @@
       <c r="DN76" s="116"/>
       <c r="DO76" s="116"/>
     </row>
-    <row r="77" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A77" s="115"/>
       <c r="B77" s="117"/>
       <c r="C77" s="116"/>
@@ -16568,7 +16567,7 @@
       <c r="DN77" s="116"/>
       <c r="DO77" s="116"/>
     </row>
-    <row r="78" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A78" s="115"/>
       <c r="B78" s="117"/>
       <c r="C78" s="116"/>
@@ -16689,7 +16688,7 @@
       <c r="DN78" s="116"/>
       <c r="DO78" s="116"/>
     </row>
-    <row r="79" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A79" s="115"/>
       <c r="B79" s="117"/>
       <c r="C79" s="116"/>
@@ -16810,7 +16809,7 @@
       <c r="DN79" s="116"/>
       <c r="DO79" s="116"/>
     </row>
-    <row r="80" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A80" s="115"/>
       <c r="B80" s="117"/>
       <c r="C80" s="116"/>
@@ -16931,7 +16930,7 @@
       <c r="DN80" s="116"/>
       <c r="DO80" s="116"/>
     </row>
-    <row r="81" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A81" s="115"/>
       <c r="B81" s="117"/>
       <c r="C81" s="116"/>
@@ -17052,7 +17051,7 @@
       <c r="DN81" s="116"/>
       <c r="DO81" s="116"/>
     </row>
-    <row r="82" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A82" s="115"/>
       <c r="B82" s="117"/>
       <c r="C82" s="116"/>
@@ -17173,7 +17172,7 @@
       <c r="DN82" s="116"/>
       <c r="DO82" s="116"/>
     </row>
-    <row r="83" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A83" s="115"/>
       <c r="B83" s="117"/>
       <c r="C83" s="116"/>
@@ -17294,7 +17293,7 @@
       <c r="DN83" s="116"/>
       <c r="DO83" s="116"/>
     </row>
-    <row r="84" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A84" s="115"/>
       <c r="B84" s="117"/>
       <c r="C84" s="116"/>
@@ -17415,7 +17414,7 @@
       <c r="DN84" s="116"/>
       <c r="DO84" s="116"/>
     </row>
-    <row r="85" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A85" s="115"/>
       <c r="B85" s="117"/>
       <c r="C85" s="116"/>
@@ -17536,7 +17535,7 @@
       <c r="DN85" s="116"/>
       <c r="DO85" s="116"/>
     </row>
-    <row r="86" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A86" s="115"/>
       <c r="B86" s="117"/>
       <c r="C86" s="116"/>
@@ -17657,7 +17656,7 @@
       <c r="DN86" s="116"/>
       <c r="DO86" s="116"/>
     </row>
-    <row r="87" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A87" s="115"/>
       <c r="B87" s="117"/>
       <c r="C87" s="116"/>
@@ -17778,7 +17777,7 @@
       <c r="DN87" s="116"/>
       <c r="DO87" s="116"/>
     </row>
-    <row r="88" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A88" s="115"/>
       <c r="B88" s="117"/>
       <c r="C88" s="116"/>
@@ -17899,7 +17898,7 @@
       <c r="DN88" s="116"/>
       <c r="DO88" s="116"/>
     </row>
-    <row r="89" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A89" s="115"/>
       <c r="B89" s="117"/>
       <c r="C89" s="116"/>
@@ -18020,7 +18019,7 @@
       <c r="DN89" s="116"/>
       <c r="DO89" s="116"/>
     </row>
-    <row r="90" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A90" s="115"/>
       <c r="B90" s="117"/>
       <c r="C90" s="116"/>
@@ -18141,7 +18140,7 @@
       <c r="DN90" s="116"/>
       <c r="DO90" s="116"/>
     </row>
-    <row r="91" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A91" s="115"/>
       <c r="B91" s="117"/>
       <c r="C91" s="116"/>
@@ -18262,7 +18261,7 @@
       <c r="DN91" s="116"/>
       <c r="DO91" s="116"/>
     </row>
-    <row r="92" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A92" s="115"/>
       <c r="B92" s="117"/>
       <c r="C92" s="116"/>
@@ -18383,7 +18382,7 @@
       <c r="DN92" s="116"/>
       <c r="DO92" s="116"/>
     </row>
-    <row r="93" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A93" s="115"/>
       <c r="B93" s="117"/>
       <c r="C93" s="116"/>
@@ -18504,7 +18503,7 @@
       <c r="DN93" s="116"/>
       <c r="DO93" s="116"/>
     </row>
-    <row r="94" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A94" s="115"/>
       <c r="B94" s="117"/>
       <c r="C94" s="116"/>
@@ -18625,7 +18624,7 @@
       <c r="DN94" s="116"/>
       <c r="DO94" s="116"/>
     </row>
-    <row r="95" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A95" s="115"/>
       <c r="B95" s="117"/>
       <c r="C95" s="116"/>
@@ -18746,7 +18745,7 @@
       <c r="DN95" s="116"/>
       <c r="DO95" s="116"/>
     </row>
-    <row r="96" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A96" s="115"/>
       <c r="B96" s="117"/>
       <c r="C96" s="116"/>
@@ -18867,7 +18866,7 @@
       <c r="DN96" s="116"/>
       <c r="DO96" s="116"/>
     </row>
-    <row r="97" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A97" s="115"/>
       <c r="B97" s="117"/>
       <c r="C97" s="116"/>
@@ -18988,7 +18987,7 @@
       <c r="DN97" s="116"/>
       <c r="DO97" s="116"/>
     </row>
-    <row r="98" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A98" s="115"/>
       <c r="B98" s="117"/>
       <c r="C98" s="116"/>
@@ -19109,7 +19108,7 @@
       <c r="DN98" s="116"/>
       <c r="DO98" s="116"/>
     </row>
-    <row r="100" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A100" s="115"/>
       <c r="B100" s="117"/>
       <c r="C100" s="116"/>
@@ -19230,7 +19229,7 @@
       <c r="DN100" s="116"/>
       <c r="DO100" s="116"/>
     </row>
-    <row r="101" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A101" s="115"/>
       <c r="B101" s="117"/>
       <c r="C101" s="116"/>
@@ -19351,7 +19350,7 @@
       <c r="DN101" s="116"/>
       <c r="DO101" s="116"/>
     </row>
-    <row r="102" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A102" s="115"/>
       <c r="B102" s="117"/>
       <c r="C102" s="116"/>
@@ -19472,7 +19471,7 @@
       <c r="DN102" s="116"/>
       <c r="DO102" s="116"/>
     </row>
-    <row r="103" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A103" s="115"/>
       <c r="B103" s="115"/>
       <c r="C103" s="116"/>
@@ -19593,7 +19592,7 @@
       <c r="DN103" s="116"/>
       <c r="DO103" s="116"/>
     </row>
-    <row r="104" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="115"/>
       <c r="B104" s="115"/>
       <c r="C104" s="116"/>
@@ -19714,7 +19713,7 @@
       <c r="DN104" s="116"/>
       <c r="DO104" s="116"/>
     </row>
-    <row r="105" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="115"/>
       <c r="B105" s="115"/>
       <c r="C105" s="116"/>
@@ -19835,7 +19834,7 @@
       <c r="DN105" s="116"/>
       <c r="DO105" s="116"/>
     </row>
-    <row r="106" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="115"/>
       <c r="B106" s="115"/>
       <c r="C106" s="116"/>
@@ -19956,7 +19955,7 @@
       <c r="DN106" s="116"/>
       <c r="DO106" s="116"/>
     </row>
-    <row r="107" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="115"/>
       <c r="B107" s="115"/>
       <c r="C107" s="116"/>
@@ -20077,7 +20076,7 @@
       <c r="DN107" s="116"/>
       <c r="DO107" s="116"/>
     </row>
-    <row r="108" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="115"/>
       <c r="B108" s="115"/>
       <c r="C108" s="116"/>
@@ -20198,7 +20197,7 @@
       <c r="DN108" s="116"/>
       <c r="DO108" s="116"/>
     </row>
-    <row r="109" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A109" s="115"/>
       <c r="B109" s="115"/>
       <c r="C109" s="116"/>
@@ -20319,7 +20318,7 @@
       <c r="DN109" s="116"/>
       <c r="DO109" s="116"/>
     </row>
-    <row r="110" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A110" s="115"/>
       <c r="B110" s="115"/>
       <c r="C110" s="116"/>
@@ -20440,7 +20439,7 @@
       <c r="DN110" s="116"/>
       <c r="DO110" s="116"/>
     </row>
-    <row r="111" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A111" s="115"/>
       <c r="B111" s="117"/>
       <c r="C111" s="116"/>
@@ -20561,7 +20560,7 @@
       <c r="DN111" s="116"/>
       <c r="DO111" s="116"/>
     </row>
-    <row r="112" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A112" s="115"/>
       <c r="B112" s="115"/>
       <c r="C112" s="116"/>
@@ -20682,7 +20681,7 @@
       <c r="DN112" s="116"/>
       <c r="DO112" s="116"/>
     </row>
-    <row r="113" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A113" s="115"/>
       <c r="B113" s="117"/>
       <c r="C113" s="116"/>
@@ -20803,7 +20802,7 @@
       <c r="DN113" s="116"/>
       <c r="DO113" s="116"/>
     </row>
-    <row r="114" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A114" s="115"/>
       <c r="B114" s="117"/>
       <c r="C114" s="116"/>
@@ -20924,7 +20923,7 @@
       <c r="DN114" s="116"/>
       <c r="DO114" s="116"/>
     </row>
-    <row r="115" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A115" s="115"/>
       <c r="B115" s="117"/>
       <c r="C115" s="116"/>
@@ -21045,7 +21044,7 @@
       <c r="DN115" s="116"/>
       <c r="DO115" s="116"/>
     </row>
-    <row r="116" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A116" s="115"/>
       <c r="B116" s="117"/>
       <c r="C116" s="116"/>
@@ -21166,7 +21165,7 @@
       <c r="DN116" s="116"/>
       <c r="DO116" s="116"/>
     </row>
-    <row r="117" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A117" s="115"/>
       <c r="B117" s="117"/>
       <c r="C117" s="116"/>
@@ -21287,7 +21286,7 @@
       <c r="DN117" s="116"/>
       <c r="DO117" s="116"/>
     </row>
-    <row r="118" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A118" s="115"/>
       <c r="B118" s="117"/>
       <c r="C118" s="116"/>
@@ -21408,7 +21407,7 @@
       <c r="DN118" s="116"/>
       <c r="DO118" s="116"/>
     </row>
-    <row r="119" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A119" s="115"/>
       <c r="B119" s="115"/>
       <c r="C119" s="116"/>
@@ -21529,7 +21528,7 @@
       <c r="DN119" s="116"/>
       <c r="DO119" s="116"/>
     </row>
-    <row r="120" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A120" s="115"/>
       <c r="B120" s="115"/>
       <c r="C120" s="116"/>
@@ -21650,7 +21649,7 @@
       <c r="DN120" s="116"/>
       <c r="DO120" s="116"/>
     </row>
-    <row r="121" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A121" s="115"/>
       <c r="B121" s="117"/>
       <c r="C121" s="116"/>
@@ -21771,7 +21770,7 @@
       <c r="DN121" s="116"/>
       <c r="DO121" s="116"/>
     </row>
-    <row r="122" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A122" s="115"/>
       <c r="B122" s="117"/>
       <c r="C122" s="116"/>
@@ -21892,7 +21891,7 @@
       <c r="DN122" s="116"/>
       <c r="DO122" s="116"/>
     </row>
-    <row r="123" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A123" s="115"/>
       <c r="B123" s="115"/>
       <c r="C123" s="116"/>
@@ -22013,7 +22012,7 @@
       <c r="DN123" s="116"/>
       <c r="DO123" s="116"/>
     </row>
-    <row r="124" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A124" s="115"/>
       <c r="B124" s="115"/>
       <c r="C124" s="116"/>
@@ -22134,7 +22133,7 @@
       <c r="DN124" s="116"/>
       <c r="DO124" s="116"/>
     </row>
-    <row r="125" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A125" s="115"/>
       <c r="B125" s="115"/>
       <c r="C125" s="116"/>
@@ -22255,7 +22254,7 @@
       <c r="DN125" s="116"/>
       <c r="DO125" s="116"/>
     </row>
-    <row r="126" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A126" s="115"/>
       <c r="B126" s="115"/>
       <c r="C126" s="116"/>
@@ -22381,14 +22380,6 @@
     <sortCondition ref="B9:B56"/>
   </sortState>
   <mergeCells count="19">
-    <mergeCell ref="CZ4:DG4"/>
-    <mergeCell ref="DH4:DO4"/>
-    <mergeCell ref="BZ4:CC4"/>
-    <mergeCell ref="CD4:CE4"/>
-    <mergeCell ref="CF4:CG4"/>
-    <mergeCell ref="CH4:CK4"/>
-    <mergeCell ref="CL4:CO4"/>
-    <mergeCell ref="CP4:CY4"/>
     <mergeCell ref="Z4:AC4"/>
     <mergeCell ref="AD4:AG4"/>
     <mergeCell ref="F4:Y4"/>
@@ -22400,6 +22391,14 @@
     <mergeCell ref="BH4:BQ4"/>
     <mergeCell ref="BR4:BS4"/>
     <mergeCell ref="BT4:BU4"/>
+    <mergeCell ref="CZ4:DG4"/>
+    <mergeCell ref="DH4:DO4"/>
+    <mergeCell ref="BZ4:CC4"/>
+    <mergeCell ref="CD4:CE4"/>
+    <mergeCell ref="CF4:CG4"/>
+    <mergeCell ref="CH4:CK4"/>
+    <mergeCell ref="CL4:CO4"/>
+    <mergeCell ref="CP4:CY4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="11" orientation="landscape" r:id="rId1"/>
@@ -22415,34 +22414,34 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="4" spans="6:20" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="4" spans="6:20" ht="15.4" x14ac:dyDescent="0.45">
       <c r="T4" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="6:20" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="5" spans="6:20" ht="15.4" x14ac:dyDescent="0.45">
       <c r="T5" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="6:20" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="6" spans="6:20" ht="15.4" x14ac:dyDescent="0.45">
       <c r="T6" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="6:20" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="7" spans="6:20" ht="15.4" x14ac:dyDescent="0.45">
       <c r="T7" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="6:20" ht="15.35" x14ac:dyDescent="0.5">
+    <row r="8" spans="6:20" ht="15.4" x14ac:dyDescent="0.45">
       <c r="T8" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="6:20" x14ac:dyDescent="0.5">
+    <row r="12" spans="6:20" x14ac:dyDescent="0.45">
       <c r="F12" t="s">
         <v>87</v>
       </c>
@@ -22462,12 +22461,12 @@
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.05859375" defaultRowHeight="13.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.05859375" style="1"/>
+    <col min="1" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:8 16384:16384" ht="41" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8 16384:16384" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>187</v>
       </c>
@@ -22493,7 +22492,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>7.4</v>
       </c>
@@ -22523,7 +22522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8 16384:16384" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8 16384:16384" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -22556,7 +22555,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8 16384:16384" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8 16384:16384" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>3.3</v>
       </c>
@@ -22585,7 +22584,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>3.3</v>
       </c>
@@ -22614,17 +22613,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M19" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M21" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="89" t="s">
         <v>191</v>
       </c>
@@ -22644,7 +22643,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="90">
         <v>42</v>
       </c>
@@ -22657,7 +22656,7 @@
         <v>3.1510472455674311E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="90">
         <v>40</v>
       </c>
@@ -22674,7 +22673,7 @@
         <v>3.5072529647841501E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="90">
         <v>38</v>
       </c>
@@ -22691,7 +22690,7 @@
         <v>5.5767506575068009E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="90">
         <v>36</v>
       </c>
@@ -22708,7 +22707,7 @@
         <v>8.8673808842062107E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="90">
         <v>34</v>
       </c>
@@ -22721,7 +22720,7 @@
         <v>2.0142411280237475E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="90">
         <v>32</v>
       </c>
@@ -22734,7 +22733,7 @@
         <v>3.2027688472636276E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="90">
         <v>30</v>
       </c>
@@ -22747,7 +22746,7 @@
         <v>5.0926019463551769E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="90">
         <v>28</v>
       </c>
@@ -22764,7 +22763,7 @@
         <v>0.56682879953465648</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="90">
         <v>26</v>
       </c>
@@ -22777,7 +22776,7 @@
         <v>0.12875615646606325</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="90">
         <v>24</v>
       </c>
@@ -22790,7 +22789,7 @@
         <v>0.20473030814712212</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="90">
         <v>22</v>
       </c>
@@ -22803,7 +22802,7 @@
         <v>0.32553394124546686</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="90">
         <v>20</v>
       </c>
@@ -22816,7 +22815,7 @@
         <v>0.51761924192803854</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="90">
         <v>18</v>
       </c>
@@ -22829,7 +22828,7 @@
         <v>0.8230468337313146</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="90">
         <v>16</v>
       </c>
@@ -22842,7 +22841,7 @@
         <v>1.3086957277552631</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="90">
         <v>14</v>
       </c>
@@ -22855,7 +22854,7 @@
         <v>2.080907717098377</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="90">
         <v>12</v>
       </c>
@@ -22885,194 +22884,194 @@
       <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.05859375" defaultRowHeight="13.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.64453125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="5.703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.64453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.64453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5859375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5859375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.64453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.76171875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="5.73046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.73046875" style="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
-    <col min="12" max="25" width="9.05859375" style="1"/>
-    <col min="26" max="26" width="10.3515625" style="1" customWidth="1"/>
-    <col min="27" max="29" width="9.05859375" style="1"/>
-    <col min="30" max="30" width="10.5859375" style="1" customWidth="1"/>
-    <col min="31" max="69" width="9.05859375" style="1"/>
-    <col min="70" max="73" width="10.64453125" style="1" customWidth="1"/>
-    <col min="74" max="81" width="9.05859375" style="1"/>
-    <col min="82" max="85" width="10.64453125" style="1" customWidth="1"/>
-    <col min="86" max="16384" width="9.05859375" style="1"/>
+    <col min="12" max="25" width="9.06640625" style="1"/>
+    <col min="26" max="26" width="10.33203125" style="1" customWidth="1"/>
+    <col min="27" max="29" width="9.06640625" style="1"/>
+    <col min="30" max="30" width="10.59765625" style="1" customWidth="1"/>
+    <col min="31" max="69" width="9.06640625" style="1"/>
+    <col min="70" max="73" width="10.6640625" style="1" customWidth="1"/>
+    <col min="74" max="81" width="9.06640625" style="1"/>
+    <col min="82" max="85" width="10.6640625" style="1" customWidth="1"/>
+    <col min="86" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:119" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:119" ht="14" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:119" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:119" ht="13.9" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:119" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="G4" s="157" t="s">
+      <c r="G4" s="151" t="s">
         <v>148</v>
       </c>
-      <c r="H4" s="159"/>
-      <c r="I4" s="154" t="s">
+      <c r="H4" s="153"/>
+      <c r="I4" s="160" t="s">
         <v>149</v>
       </c>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="155"/>
-      <c r="M4" s="155"/>
-      <c r="N4" s="155"/>
-      <c r="O4" s="155"/>
-      <c r="P4" s="155"/>
-      <c r="Q4" s="155"/>
-      <c r="R4" s="155"/>
-      <c r="S4" s="155"/>
-      <c r="T4" s="155"/>
-      <c r="U4" s="155"/>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
-      <c r="Z4" s="151" t="s">
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
+      <c r="L4" s="161"/>
+      <c r="M4" s="161"/>
+      <c r="N4" s="161"/>
+      <c r="O4" s="161"/>
+      <c r="P4" s="161"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="161"/>
+      <c r="S4" s="161"/>
+      <c r="T4" s="161"/>
+      <c r="U4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
+      <c r="Z4" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="AA4" s="152"/>
-      <c r="AB4" s="152"/>
-      <c r="AC4" s="153"/>
-      <c r="AD4" s="151" t="s">
+      <c r="AA4" s="158"/>
+      <c r="AB4" s="158"/>
+      <c r="AC4" s="159"/>
+      <c r="AD4" s="157" t="s">
         <v>151</v>
       </c>
-      <c r="AE4" s="152"/>
-      <c r="AF4" s="152"/>
-      <c r="AG4" s="153"/>
-      <c r="AH4" s="157" t="s">
+      <c r="AE4" s="158"/>
+      <c r="AF4" s="158"/>
+      <c r="AG4" s="159"/>
+      <c r="AH4" s="151" t="s">
         <v>152</v>
       </c>
-      <c r="AI4" s="158"/>
-      <c r="AJ4" s="158"/>
-      <c r="AK4" s="158"/>
-      <c r="AL4" s="158"/>
-      <c r="AM4" s="160"/>
-      <c r="AN4" s="161" t="s">
+      <c r="AI4" s="152"/>
+      <c r="AJ4" s="152"/>
+      <c r="AK4" s="152"/>
+      <c r="AL4" s="152"/>
+      <c r="AM4" s="155"/>
+      <c r="AN4" s="156" t="s">
         <v>153</v>
       </c>
-      <c r="AO4" s="158"/>
-      <c r="AP4" s="158"/>
-      <c r="AQ4" s="158"/>
-      <c r="AR4" s="158"/>
-      <c r="AS4" s="158"/>
-      <c r="AT4" s="158"/>
-      <c r="AU4" s="158"/>
-      <c r="AV4" s="158"/>
-      <c r="AW4" s="159"/>
-      <c r="AX4" s="157" t="s">
+      <c r="AO4" s="152"/>
+      <c r="AP4" s="152"/>
+      <c r="AQ4" s="152"/>
+      <c r="AR4" s="152"/>
+      <c r="AS4" s="152"/>
+      <c r="AT4" s="152"/>
+      <c r="AU4" s="152"/>
+      <c r="AV4" s="152"/>
+      <c r="AW4" s="153"/>
+      <c r="AX4" s="151" t="s">
         <v>154</v>
       </c>
-      <c r="AY4" s="158"/>
-      <c r="AZ4" s="158"/>
-      <c r="BA4" s="158"/>
-      <c r="BB4" s="158"/>
-      <c r="BC4" s="158"/>
-      <c r="BD4" s="158"/>
-      <c r="BE4" s="158"/>
-      <c r="BF4" s="158"/>
-      <c r="BG4" s="159"/>
-      <c r="BH4" s="157" t="s">
+      <c r="AY4" s="152"/>
+      <c r="AZ4" s="152"/>
+      <c r="BA4" s="152"/>
+      <c r="BB4" s="152"/>
+      <c r="BC4" s="152"/>
+      <c r="BD4" s="152"/>
+      <c r="BE4" s="152"/>
+      <c r="BF4" s="152"/>
+      <c r="BG4" s="153"/>
+      <c r="BH4" s="151" t="s">
         <v>155</v>
       </c>
-      <c r="BI4" s="158"/>
-      <c r="BJ4" s="158"/>
-      <c r="BK4" s="158"/>
-      <c r="BL4" s="158"/>
-      <c r="BM4" s="158"/>
-      <c r="BN4" s="158"/>
-      <c r="BO4" s="158"/>
-      <c r="BP4" s="158"/>
-      <c r="BQ4" s="159"/>
-      <c r="BR4" s="157" t="s">
+      <c r="BI4" s="152"/>
+      <c r="BJ4" s="152"/>
+      <c r="BK4" s="152"/>
+      <c r="BL4" s="152"/>
+      <c r="BM4" s="152"/>
+      <c r="BN4" s="152"/>
+      <c r="BO4" s="152"/>
+      <c r="BP4" s="152"/>
+      <c r="BQ4" s="153"/>
+      <c r="BR4" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="BS4" s="160"/>
-      <c r="BT4" s="161" t="s">
+      <c r="BS4" s="155"/>
+      <c r="BT4" s="156" t="s">
         <v>157</v>
       </c>
-      <c r="BU4" s="159"/>
-      <c r="BV4" s="157" t="s">
+      <c r="BU4" s="153"/>
+      <c r="BV4" s="151" t="s">
         <v>160</v>
       </c>
-      <c r="BW4" s="158"/>
-      <c r="BX4" s="158"/>
-      <c r="BY4" s="159"/>
-      <c r="BZ4" s="157" t="s">
+      <c r="BW4" s="152"/>
+      <c r="BX4" s="152"/>
+      <c r="BY4" s="153"/>
+      <c r="BZ4" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="CA4" s="158"/>
-      <c r="CB4" s="158"/>
-      <c r="CC4" s="159"/>
-      <c r="CD4" s="157" t="s">
+      <c r="CA4" s="152"/>
+      <c r="CB4" s="152"/>
+      <c r="CC4" s="153"/>
+      <c r="CD4" s="151" t="s">
         <v>158</v>
       </c>
-      <c r="CE4" s="160"/>
-      <c r="CF4" s="161" t="s">
+      <c r="CE4" s="155"/>
+      <c r="CF4" s="156" t="s">
         <v>159</v>
       </c>
-      <c r="CG4" s="159"/>
-      <c r="CH4" s="157" t="s">
+      <c r="CG4" s="153"/>
+      <c r="CH4" s="151" t="s">
         <v>162</v>
       </c>
-      <c r="CI4" s="158"/>
-      <c r="CJ4" s="158"/>
-      <c r="CK4" s="159"/>
-      <c r="CL4" s="157" t="s">
+      <c r="CI4" s="152"/>
+      <c r="CJ4" s="152"/>
+      <c r="CK4" s="153"/>
+      <c r="CL4" s="151" t="s">
         <v>163</v>
       </c>
-      <c r="CM4" s="158"/>
-      <c r="CN4" s="158"/>
-      <c r="CO4" s="159"/>
-      <c r="CP4" s="157" t="s">
+      <c r="CM4" s="152"/>
+      <c r="CN4" s="152"/>
+      <c r="CO4" s="153"/>
+      <c r="CP4" s="151" t="s">
         <v>164</v>
       </c>
-      <c r="CQ4" s="158"/>
-      <c r="CR4" s="158"/>
-      <c r="CS4" s="158"/>
-      <c r="CT4" s="158"/>
-      <c r="CU4" s="158"/>
-      <c r="CV4" s="158"/>
-      <c r="CW4" s="158"/>
-      <c r="CX4" s="158"/>
-      <c r="CY4" s="159"/>
-      <c r="CZ4" s="157" t="s">
+      <c r="CQ4" s="152"/>
+      <c r="CR4" s="152"/>
+      <c r="CS4" s="152"/>
+      <c r="CT4" s="152"/>
+      <c r="CU4" s="152"/>
+      <c r="CV4" s="152"/>
+      <c r="CW4" s="152"/>
+      <c r="CX4" s="152"/>
+      <c r="CY4" s="153"/>
+      <c r="CZ4" s="151" t="s">
         <v>165</v>
       </c>
-      <c r="DA4" s="158"/>
-      <c r="DB4" s="158"/>
-      <c r="DC4" s="158"/>
-      <c r="DD4" s="158"/>
-      <c r="DE4" s="158"/>
-      <c r="DF4" s="158"/>
-      <c r="DG4" s="159"/>
-      <c r="DH4" s="157" t="s">
+      <c r="DA4" s="152"/>
+      <c r="DB4" s="152"/>
+      <c r="DC4" s="152"/>
+      <c r="DD4" s="152"/>
+      <c r="DE4" s="152"/>
+      <c r="DF4" s="152"/>
+      <c r="DG4" s="153"/>
+      <c r="DH4" s="151" t="s">
         <v>178</v>
       </c>
-      <c r="DI4" s="158"/>
-      <c r="DJ4" s="158"/>
-      <c r="DK4" s="158"/>
-      <c r="DL4" s="158"/>
-      <c r="DM4" s="158"/>
-      <c r="DN4" s="158"/>
-      <c r="DO4" s="159"/>
+      <c r="DI4" s="152"/>
+      <c r="DJ4" s="152"/>
+      <c r="DK4" s="152"/>
+      <c r="DL4" s="152"/>
+      <c r="DM4" s="152"/>
+      <c r="DN4" s="152"/>
+      <c r="DO4" s="153"/>
     </row>
-    <row r="5" spans="1:119" ht="72.349999999999994" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:119" ht="70.900000000000006" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
@@ -23422,7 +23421,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
@@ -23769,7 +23768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
@@ -24092,7 +24091,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:119" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:119" ht="49.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
@@ -24451,7 +24450,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:119" ht="55" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:119" ht="54.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="45" t="s">
         <v>147</v>
       </c>
@@ -24582,8 +24581,8 @@
       <c r="DN9" s="81"/>
       <c r="DO9" s="82"/>
     </row>
-    <row r="10" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="166" t="s">
+    <row r="10" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="163" t="s">
         <v>148</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -24713,8 +24712,8 @@
       <c r="DN10" s="83"/>
       <c r="DO10" s="84"/>
     </row>
-    <row r="11" spans="1:119" ht="27.7" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="167"/>
+    <row r="11" spans="1:119" ht="27.4" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="165"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17">
         <v>2</v>
@@ -24840,8 +24839,8 @@
       <c r="DN11" s="83"/>
       <c r="DO11" s="84"/>
     </row>
-    <row r="12" spans="1:119" ht="41.35" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="163" t="s">
+    <row r="12" spans="1:119" ht="40.9" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="166" t="s">
         <v>149</v>
       </c>
       <c r="B12" s="47" t="s">
@@ -24971,7 +24970,7 @@
       <c r="DN12" s="83"/>
       <c r="DO12" s="84"/>
     </row>
-    <row r="13" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A13" s="164"/>
       <c r="B13" s="16" t="s">
         <v>5</v>
@@ -25100,7 +25099,7 @@
       <c r="DN13" s="83"/>
       <c r="DO13" s="84"/>
     </row>
-    <row r="14" spans="1:119" ht="43.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:119" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="164"/>
       <c r="B14" s="16" t="s">
         <v>35</v>
@@ -25231,7 +25230,7 @@
       <c r="DN14" s="83"/>
       <c r="DO14" s="84"/>
     </row>
-    <row r="15" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A15" s="164"/>
       <c r="B15" s="16" t="s">
         <v>8</v>
@@ -25360,7 +25359,7 @@
       <c r="DN15" s="83"/>
       <c r="DO15" s="84"/>
     </row>
-    <row r="16" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A16" s="164"/>
       <c r="B16" s="16" t="s">
         <v>30</v>
@@ -25489,7 +25488,7 @@
       <c r="DN16" s="83"/>
       <c r="DO16" s="84"/>
     </row>
-    <row r="17" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A17" s="164"/>
       <c r="B17" s="16" t="s">
         <v>31</v>
@@ -25618,7 +25617,7 @@
       <c r="DN17" s="83"/>
       <c r="DO17" s="84"/>
     </row>
-    <row r="18" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A18" s="164"/>
       <c r="B18" s="16" t="s">
         <v>32</v>
@@ -25747,7 +25746,7 @@
       <c r="DN18" s="83"/>
       <c r="DO18" s="84"/>
     </row>
-    <row r="19" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A19" s="164"/>
       <c r="B19" s="16" t="s">
         <v>22</v>
@@ -25876,7 +25875,7 @@
       <c r="DN19" s="83"/>
       <c r="DO19" s="84"/>
     </row>
-    <row r="20" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A20" s="164"/>
       <c r="B20" s="16" t="s">
         <v>23</v>
@@ -26005,7 +26004,7 @@
       <c r="DN20" s="83"/>
       <c r="DO20" s="84"/>
     </row>
-    <row r="21" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A21" s="164"/>
       <c r="B21" s="16" t="s">
         <v>24</v>
@@ -26134,7 +26133,7 @@
       <c r="DN21" s="83"/>
       <c r="DO21" s="84"/>
     </row>
-    <row r="22" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A22" s="164"/>
       <c r="B22" s="16" t="s">
         <v>25</v>
@@ -26263,7 +26262,7 @@
       <c r="DN22" s="83"/>
       <c r="DO22" s="84"/>
     </row>
-    <row r="23" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A23" s="164"/>
       <c r="B23" s="16" t="s">
         <v>26</v>
@@ -26392,7 +26391,7 @@
       <c r="DN23" s="83"/>
       <c r="DO23" s="84"/>
     </row>
-    <row r="24" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A24" s="164"/>
       <c r="B24" s="16" t="s">
         <v>27</v>
@@ -26521,7 +26520,7 @@
       <c r="DN24" s="83"/>
       <c r="DO24" s="84"/>
     </row>
-    <row r="25" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A25" s="164"/>
       <c r="B25" s="16" t="s">
         <v>28</v>
@@ -26650,7 +26649,7 @@
       <c r="DN25" s="83"/>
       <c r="DO25" s="84"/>
     </row>
-    <row r="26" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A26" s="164"/>
       <c r="B26" s="16" t="s">
         <v>29</v>
@@ -26779,7 +26778,7 @@
       <c r="DN26" s="83"/>
       <c r="DO26" s="84"/>
     </row>
-    <row r="27" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A27" s="164"/>
       <c r="B27" s="16" t="s">
         <v>45</v>
@@ -26908,8 +26907,8 @@
       <c r="DN27" s="83"/>
       <c r="DO27" s="84"/>
     </row>
-    <row r="28" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="165"/>
+    <row r="28" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="167"/>
       <c r="B28" s="50" t="s">
         <v>46</v>
       </c>
@@ -27037,8 +27036,8 @@
       <c r="DN28" s="83"/>
       <c r="DO28" s="84"/>
     </row>
-    <row r="29" spans="1:119" ht="55" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="166" t="s">
+    <row r="29" spans="1:119" ht="54.4" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="163" t="s">
         <v>150</v>
       </c>
       <c r="B29" s="15" t="s">
@@ -27168,7 +27167,7 @@
       <c r="DN29" s="83"/>
       <c r="DO29" s="84"/>
     </row>
-    <row r="30" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A30" s="164"/>
       <c r="B30" s="16" t="s">
         <v>37</v>
@@ -27297,7 +27296,7 @@
       <c r="DN30" s="83"/>
       <c r="DO30" s="84"/>
     </row>
-    <row r="31" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A31" s="164"/>
       <c r="B31" s="16" t="s">
         <v>38</v>
@@ -27428,8 +27427,8 @@
       <c r="DN31" s="83"/>
       <c r="DO31" s="84"/>
     </row>
-    <row r="32" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="167"/>
+    <row r="32" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="165"/>
       <c r="B32" s="17" t="s">
         <v>39</v>
       </c>
@@ -27557,8 +27556,8 @@
       <c r="DN32" s="83"/>
       <c r="DO32" s="84"/>
     </row>
-    <row r="33" spans="1:119" ht="55" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="163" t="s">
+    <row r="33" spans="1:119" ht="54.4" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="166" t="s">
         <v>151</v>
       </c>
       <c r="B33" s="48" t="s">
@@ -27688,7 +27687,7 @@
       <c r="DN33" s="83"/>
       <c r="DO33" s="84"/>
     </row>
-    <row r="34" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A34" s="164"/>
       <c r="B34" s="16" t="s">
         <v>37</v>
@@ -27817,7 +27816,7 @@
       <c r="DN34" s="83"/>
       <c r="DO34" s="84"/>
     </row>
-    <row r="35" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A35" s="164"/>
       <c r="B35" s="16" t="s">
         <v>38</v>
@@ -27948,8 +27947,8 @@
       <c r="DN35" s="83"/>
       <c r="DO35" s="84"/>
     </row>
-    <row r="36" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="165"/>
+    <row r="36" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="167"/>
       <c r="B36" s="50" t="s">
         <v>39</v>
       </c>
@@ -28077,8 +28076,8 @@
       <c r="DN36" s="83"/>
       <c r="DO36" s="84"/>
     </row>
-    <row r="37" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="166" t="s">
+    <row r="37" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="163" t="s">
         <v>152</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -28208,7 +28207,7 @@
       <c r="DN37" s="83"/>
       <c r="DO37" s="84"/>
     </row>
-    <row r="38" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A38" s="164"/>
       <c r="B38" s="16" t="s">
         <v>56</v>
@@ -28337,7 +28336,7 @@
       <c r="DN38" s="83"/>
       <c r="DO38" s="84"/>
     </row>
-    <row r="39" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A39" s="164"/>
       <c r="B39" s="16" t="s">
         <v>56</v>
@@ -28466,7 +28465,7 @@
       <c r="DN39" s="83"/>
       <c r="DO39" s="84"/>
     </row>
-    <row r="40" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A40" s="164"/>
       <c r="B40" s="16" t="s">
         <v>56</v>
@@ -28597,7 +28596,7 @@
       <c r="DN40" s="83"/>
       <c r="DO40" s="84"/>
     </row>
-    <row r="41" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A41" s="164"/>
       <c r="B41" s="16" t="s">
         <v>56</v>
@@ -28726,8 +28725,8 @@
       <c r="DN41" s="83"/>
       <c r="DO41" s="84"/>
     </row>
-    <row r="42" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="167"/>
+    <row r="42" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="165"/>
       <c r="B42" s="17" t="s">
         <v>56</v>
       </c>
@@ -28855,8 +28854,8 @@
       <c r="DN42" s="83"/>
       <c r="DO42" s="84"/>
     </row>
-    <row r="43" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="163" t="s">
+    <row r="43" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="166" t="s">
         <v>153</v>
       </c>
       <c r="B43" s="48" t="s">
@@ -28988,7 +28987,7 @@
       <c r="DN43" s="83"/>
       <c r="DO43" s="84"/>
     </row>
-    <row r="44" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A44" s="164"/>
       <c r="B44" s="16" t="s">
         <v>56</v>
@@ -29119,7 +29118,7 @@
       <c r="DN44" s="83"/>
       <c r="DO44" s="84"/>
     </row>
-    <row r="45" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A45" s="164"/>
       <c r="B45" s="16" t="s">
         <v>56</v>
@@ -29248,7 +29247,7 @@
       <c r="DN45" s="83"/>
       <c r="DO45" s="84"/>
     </row>
-    <row r="46" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A46" s="164"/>
       <c r="B46" s="16" t="s">
         <v>56</v>
@@ -29377,7 +29376,7 @@
       <c r="DN46" s="83"/>
       <c r="DO46" s="84"/>
     </row>
-    <row r="47" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A47" s="164"/>
       <c r="B47" s="16" t="s">
         <v>56</v>
@@ -29506,7 +29505,7 @@
       <c r="DN47" s="83"/>
       <c r="DO47" s="84"/>
     </row>
-    <row r="48" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A48" s="164"/>
       <c r="B48" s="16" t="s">
         <v>56</v>
@@ -29635,7 +29634,7 @@
       <c r="DN48" s="83"/>
       <c r="DO48" s="84"/>
     </row>
-    <row r="49" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A49" s="164"/>
       <c r="B49" s="16" t="s">
         <v>56</v>
@@ -29764,7 +29763,7 @@
       <c r="DN49" s="83"/>
       <c r="DO49" s="84"/>
     </row>
-    <row r="50" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A50" s="164"/>
       <c r="B50" s="16" t="s">
         <v>56</v>
@@ -29893,7 +29892,7 @@
       <c r="DN50" s="83"/>
       <c r="DO50" s="84"/>
     </row>
-    <row r="51" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A51" s="164"/>
       <c r="B51" s="16" t="s">
         <v>56</v>
@@ -30022,8 +30021,8 @@
       <c r="DN51" s="83"/>
       <c r="DO51" s="84"/>
     </row>
-    <row r="52" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="165"/>
+    <row r="52" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="167"/>
       <c r="B52" s="50" t="s">
         <v>56</v>
       </c>
@@ -30151,8 +30150,8 @@
       <c r="DN52" s="83"/>
       <c r="DO52" s="84"/>
     </row>
-    <row r="53" spans="1:119" ht="54.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="166" t="s">
+    <row r="53" spans="1:119" ht="54.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="163" t="s">
         <v>154</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -30280,7 +30279,7 @@
       <c r="DN53" s="83"/>
       <c r="DO53" s="84"/>
     </row>
-    <row r="54" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A54" s="164"/>
       <c r="B54" s="16" t="s">
         <v>71</v>
@@ -30407,7 +30406,7 @@
       <c r="DN54" s="83"/>
       <c r="DO54" s="84"/>
     </row>
-    <row r="55" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A55" s="164"/>
       <c r="B55" s="16" t="s">
         <v>72</v>
@@ -30534,7 +30533,7 @@
       <c r="DN55" s="83"/>
       <c r="DO55" s="84"/>
     </row>
-    <row r="56" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A56" s="164"/>
       <c r="B56" s="16" t="s">
         <v>73</v>
@@ -30661,7 +30660,7 @@
       <c r="DN56" s="83"/>
       <c r="DO56" s="84"/>
     </row>
-    <row r="57" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A57" s="164"/>
       <c r="B57" s="16" t="s">
         <v>74</v>
@@ -30788,7 +30787,7 @@
       <c r="DN57" s="83"/>
       <c r="DO57" s="84"/>
     </row>
-    <row r="58" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A58" s="164"/>
       <c r="B58" s="16" t="s">
         <v>75</v>
@@ -30915,7 +30914,7 @@
       <c r="DN58" s="83"/>
       <c r="DO58" s="84"/>
     </row>
-    <row r="59" spans="1:119" ht="82" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:119" ht="81" x14ac:dyDescent="0.35">
       <c r="A59" s="164"/>
       <c r="B59" s="16" t="s">
         <v>76</v>
@@ -31046,7 +31045,7 @@
       <c r="DN59" s="83"/>
       <c r="DO59" s="84"/>
     </row>
-    <row r="60" spans="1:119" ht="82" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:119" ht="81" x14ac:dyDescent="0.35">
       <c r="A60" s="164"/>
       <c r="B60" s="16" t="s">
         <v>77</v>
@@ -31177,7 +31176,7 @@
       <c r="DN60" s="83"/>
       <c r="DO60" s="84"/>
     </row>
-    <row r="61" spans="1:119" ht="95.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:119" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A61" s="164"/>
       <c r="B61" s="16" t="s">
         <v>78</v>
@@ -31308,8 +31307,8 @@
       <c r="DN61" s="83"/>
       <c r="DO61" s="84"/>
     </row>
-    <row r="62" spans="1:119" ht="96" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="167"/>
+    <row r="62" spans="1:119" ht="94.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="165"/>
       <c r="B62" s="17" t="s">
         <v>79</v>
       </c>
@@ -31439,8 +31438,8 @@
       <c r="DN62" s="83"/>
       <c r="DO62" s="84"/>
     </row>
-    <row r="63" spans="1:119" ht="54.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="163" t="s">
+    <row r="63" spans="1:119" ht="54.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="166" t="s">
         <v>155</v>
       </c>
       <c r="B63" s="48" t="s">
@@ -31568,7 +31567,7 @@
       <c r="DN63" s="83"/>
       <c r="DO63" s="84"/>
     </row>
-    <row r="64" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A64" s="164"/>
       <c r="B64" s="16" t="s">
         <v>71</v>
@@ -31695,7 +31694,7 @@
       <c r="DN64" s="83"/>
       <c r="DO64" s="84"/>
     </row>
-    <row r="65" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A65" s="164"/>
       <c r="B65" s="16" t="s">
         <v>72</v>
@@ -31822,7 +31821,7 @@
       <c r="DN65" s="83"/>
       <c r="DO65" s="84"/>
     </row>
-    <row r="66" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A66" s="164"/>
       <c r="B66" s="16" t="s">
         <v>73</v>
@@ -31949,7 +31948,7 @@
       <c r="DN66" s="83"/>
       <c r="DO66" s="84"/>
     </row>
-    <row r="67" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A67" s="164"/>
       <c r="B67" s="16" t="s">
         <v>74</v>
@@ -32076,7 +32075,7 @@
       <c r="DN67" s="83"/>
       <c r="DO67" s="84"/>
     </row>
-    <row r="68" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:119" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A68" s="164"/>
       <c r="B68" s="16" t="s">
         <v>75</v>
@@ -32203,7 +32202,7 @@
       <c r="DN68" s="83"/>
       <c r="DO68" s="84"/>
     </row>
-    <row r="69" spans="1:119" ht="68.349999999999994" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:119" ht="81" x14ac:dyDescent="0.35">
       <c r="A69" s="164"/>
       <c r="B69" s="16" t="s">
         <v>76</v>
@@ -32334,7 +32333,7 @@
       <c r="DN69" s="83"/>
       <c r="DO69" s="84"/>
     </row>
-    <row r="70" spans="1:119" ht="82" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:119" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A70" s="164"/>
       <c r="B70" s="16" t="s">
         <v>77</v>
@@ -32465,7 +32464,7 @@
       <c r="DN70" s="83"/>
       <c r="DO70" s="84"/>
     </row>
-    <row r="71" spans="1:119" ht="82" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:119" ht="81" x14ac:dyDescent="0.35">
       <c r="A71" s="164"/>
       <c r="B71" s="16" t="s">
         <v>78</v>
@@ -32596,8 +32595,8 @@
       <c r="DN71" s="83"/>
       <c r="DO71" s="84"/>
     </row>
-    <row r="72" spans="1:119" ht="96" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="165"/>
+    <row r="72" spans="1:119" ht="94.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="167"/>
       <c r="B72" s="50" t="s">
         <v>79</v>
       </c>
@@ -32727,8 +32726,8 @@
       <c r="DN72" s="83"/>
       <c r="DO72" s="84"/>
     </row>
-    <row r="73" spans="1:119" ht="41.35" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="166" t="s">
+    <row r="73" spans="1:119" ht="40.9" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="163" t="s">
         <v>156</v>
       </c>
       <c r="B73" s="15" t="s">
@@ -32858,8 +32857,8 @@
       <c r="DN73" s="83"/>
       <c r="DO73" s="84"/>
     </row>
-    <row r="74" spans="1:119" ht="55" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="167"/>
+    <row r="74" spans="1:119" ht="67.900000000000006" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="165"/>
       <c r="B74" s="17" t="s">
         <v>67</v>
       </c>
@@ -32987,8 +32986,8 @@
       <c r="DN74" s="83"/>
       <c r="DO74" s="84"/>
     </row>
-    <row r="75" spans="1:119" ht="41.35" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="163" t="s">
+    <row r="75" spans="1:119" ht="40.9" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="166" t="s">
         <v>157</v>
       </c>
       <c r="B75" s="48" t="s">
@@ -33118,8 +33117,8 @@
       <c r="DN75" s="83"/>
       <c r="DO75" s="84"/>
     </row>
-    <row r="76" spans="1:119" ht="55" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="165"/>
+    <row r="76" spans="1:119" ht="67.900000000000006" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="167"/>
       <c r="B76" s="50" t="s">
         <v>67</v>
       </c>
@@ -33247,8 +33246,8 @@
       <c r="DN76" s="83"/>
       <c r="DO76" s="84"/>
     </row>
-    <row r="77" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="166" t="s">
+    <row r="77" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="163" t="s">
         <v>160</v>
       </c>
       <c r="B77" s="15" t="s">
@@ -33378,7 +33377,7 @@
       <c r="DN77" s="83"/>
       <c r="DO77" s="84"/>
     </row>
-    <row r="78" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A78" s="164"/>
       <c r="B78" s="16" t="s">
         <v>80</v>
@@ -33507,7 +33506,7 @@
       <c r="DN78" s="83"/>
       <c r="DO78" s="84"/>
     </row>
-    <row r="79" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A79" s="164"/>
       <c r="B79" s="16" t="s">
         <v>112</v>
@@ -33636,8 +33635,8 @@
       <c r="DN79" s="83"/>
       <c r="DO79" s="84"/>
     </row>
-    <row r="80" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="167"/>
+    <row r="80" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="165"/>
       <c r="B80" s="17" t="s">
         <v>113</v>
       </c>
@@ -33765,8 +33764,8 @@
       <c r="DN80" s="83"/>
       <c r="DO80" s="84"/>
     </row>
-    <row r="81" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="163" t="s">
+    <row r="81" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="166" t="s">
         <v>161</v>
       </c>
       <c r="B81" s="48" t="s">
@@ -33896,7 +33895,7 @@
       <c r="DN81" s="83"/>
       <c r="DO81" s="84"/>
     </row>
-    <row r="82" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A82" s="164"/>
       <c r="B82" s="16" t="s">
         <v>80</v>
@@ -34025,7 +34024,7 @@
       <c r="DN82" s="83"/>
       <c r="DO82" s="84"/>
     </row>
-    <row r="83" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A83" s="164"/>
       <c r="B83" s="16" t="s">
         <v>112</v>
@@ -34154,8 +34153,8 @@
       <c r="DN83" s="83"/>
       <c r="DO83" s="84"/>
     </row>
-    <row r="84" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="165"/>
+    <row r="84" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="167"/>
       <c r="B84" s="50" t="s">
         <v>113</v>
       </c>
@@ -34283,8 +34282,8 @@
       <c r="DN84" s="83"/>
       <c r="DO84" s="84"/>
     </row>
-    <row r="85" spans="1:119" ht="41.35" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="166" t="s">
+    <row r="85" spans="1:119" ht="40.9" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="163" t="s">
         <v>158</v>
       </c>
       <c r="B85" s="15" t="s">
@@ -34414,8 +34413,8 @@
       <c r="DN85" s="83"/>
       <c r="DO85" s="84"/>
     </row>
-    <row r="86" spans="1:119" ht="68.7" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="167"/>
+    <row r="86" spans="1:119" ht="67.900000000000006" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="165"/>
       <c r="B86" s="17" t="s">
         <v>67</v>
       </c>
@@ -34543,8 +34542,8 @@
       <c r="DN86" s="83"/>
       <c r="DO86" s="84"/>
     </row>
-    <row r="87" spans="1:119" ht="41.35" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="163" t="s">
+    <row r="87" spans="1:119" ht="40.9" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="166" t="s">
         <v>159</v>
       </c>
       <c r="B87" s="48" t="s">
@@ -34674,8 +34673,8 @@
       <c r="DN87" s="83"/>
       <c r="DO87" s="84"/>
     </row>
-    <row r="88" spans="1:119" ht="68.7" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="165"/>
+    <row r="88" spans="1:119" ht="67.900000000000006" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="167"/>
       <c r="B88" s="50" t="s">
         <v>67</v>
       </c>
@@ -34803,8 +34802,8 @@
       <c r="DN88" s="83"/>
       <c r="DO88" s="84"/>
     </row>
-    <row r="89" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="166" t="s">
+    <row r="89" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="163" t="s">
         <v>162</v>
       </c>
       <c r="B89" s="15" t="s">
@@ -34934,7 +34933,7 @@
       <c r="DN89" s="83"/>
       <c r="DO89" s="84"/>
     </row>
-    <row r="90" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A90" s="164"/>
       <c r="B90" s="16" t="s">
         <v>80</v>
@@ -35063,7 +35062,7 @@
       <c r="DN90" s="83"/>
       <c r="DO90" s="84"/>
     </row>
-    <row r="91" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A91" s="164"/>
       <c r="B91" s="16" t="s">
         <v>112</v>
@@ -35192,8 +35191,8 @@
       <c r="DN91" s="83"/>
       <c r="DO91" s="84"/>
     </row>
-    <row r="92" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="167"/>
+    <row r="92" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="165"/>
       <c r="B92" s="39" t="s">
         <v>113</v>
       </c>
@@ -35321,8 +35320,8 @@
       <c r="DN92" s="83"/>
       <c r="DO92" s="84"/>
     </row>
-    <row r="93" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="163" t="s">
+    <row r="93" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="166" t="s">
         <v>163</v>
       </c>
       <c r="B93" s="48" t="s">
@@ -35452,7 +35451,7 @@
       <c r="DN93" s="83"/>
       <c r="DO93" s="84"/>
     </row>
-    <row r="94" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A94" s="164"/>
       <c r="B94" s="16" t="s">
         <v>80</v>
@@ -35581,7 +35580,7 @@
       <c r="DN94" s="83"/>
       <c r="DO94" s="84"/>
     </row>
-    <row r="95" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A95" s="164"/>
       <c r="B95" s="16" t="s">
         <v>112</v>
@@ -35710,8 +35709,8 @@
       <c r="DN95" s="83"/>
       <c r="DO95" s="84"/>
     </row>
-    <row r="96" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="165"/>
+    <row r="96" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="167"/>
       <c r="B96" s="53" t="s">
         <v>113</v>
       </c>
@@ -35839,8 +35838,8 @@
       <c r="DN96" s="83"/>
       <c r="DO96" s="84"/>
     </row>
-    <row r="97" spans="1:119" ht="40.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="166" t="s">
+    <row r="97" spans="1:119" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="163" t="s">
         <v>164</v>
       </c>
       <c r="B97" s="15" t="s">
@@ -35970,7 +35969,7 @@
       <c r="DN97" s="83"/>
       <c r="DO97" s="84"/>
     </row>
-    <row r="98" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A98" s="164"/>
       <c r="B98" s="36" t="s">
         <v>130</v>
@@ -36099,7 +36098,7 @@
       <c r="DN98" s="83"/>
       <c r="DO98" s="84"/>
     </row>
-    <row r="99" spans="1:119" ht="27.35" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:119" ht="27" x14ac:dyDescent="0.35">
       <c r="A99" s="164"/>
       <c r="B99" s="16" t="s">
         <v>80</v>
@@ -36228,7 +36227,7 @@
       <c r="DN99" s="83"/>
       <c r="DO99" s="84"/>
     </row>
-    <row r="100" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="164"/>
       <c r="B100" s="16" t="s">
         <v>131</v>
@@ -36357,7 +36356,7 @@
       <c r="DN100" s="83"/>
       <c r="DO100" s="84"/>
     </row>
-    <row r="101" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="164"/>
       <c r="B101" s="16" t="s">
         <v>132</v>
@@ -36486,7 +36485,7 @@
       <c r="DN101" s="83"/>
       <c r="DO101" s="84"/>
     </row>
-    <row r="102" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="164"/>
       <c r="B102" s="16" t="s">
         <v>133</v>
@@ -36615,7 +36614,7 @@
       <c r="DN102" s="83"/>
       <c r="DO102" s="84"/>
     </row>
-    <row r="103" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="164"/>
       <c r="B103" s="36" t="s">
         <v>134</v>
@@ -36744,7 +36743,7 @@
       <c r="DN103" s="83"/>
       <c r="DO103" s="84"/>
     </row>
-    <row r="104" spans="1:119" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:119" ht="14.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="164"/>
       <c r="B104" s="36" t="s">
         <v>135</v>
@@ -36873,7 +36872,7 @@
       <c r="DN104" s="83"/>
       <c r="DO104" s="84"/>
     </row>
-    <row r="105" spans="1:119" ht="27.35" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:119" ht="27" x14ac:dyDescent="0.35">
       <c r="A105" s="164"/>
       <c r="B105" s="36" t="s">
         <v>136</v>
@@ -37002,8 +37001,8 @@
       <c r="DN105" s="83"/>
       <c r="DO105" s="84"/>
     </row>
-    <row r="106" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A106" s="167"/>
+    <row r="106" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="165"/>
       <c r="B106" s="39" t="s">
         <v>137</v>
       </c>
@@ -37131,8 +37130,8 @@
       <c r="DN106" s="83"/>
       <c r="DO106" s="84"/>
     </row>
-    <row r="107" spans="1:119" ht="55" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="163" t="s">
+    <row r="107" spans="1:119" ht="54.4" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="166" t="s">
         <v>165</v>
       </c>
       <c r="B107" s="48" t="s">
@@ -37262,7 +37261,7 @@
       <c r="DN107" s="83"/>
       <c r="DO107" s="84"/>
     </row>
-    <row r="108" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A108" s="164"/>
       <c r="B108" s="16" t="s">
         <v>56</v>
@@ -37391,7 +37390,7 @@
       <c r="DN108" s="83"/>
       <c r="DO108" s="84"/>
     </row>
-    <row r="109" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A109" s="164"/>
       <c r="B109" s="16" t="s">
         <v>56</v>
@@ -37520,7 +37519,7 @@
       <c r="DN109" s="83"/>
       <c r="DO109" s="84"/>
     </row>
-    <row r="110" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A110" s="164"/>
       <c r="B110" s="16" t="s">
         <v>56</v>
@@ -37649,7 +37648,7 @@
       <c r="DN110" s="83"/>
       <c r="DO110" s="84"/>
     </row>
-    <row r="111" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A111" s="164"/>
       <c r="B111" s="16" t="s">
         <v>56</v>
@@ -37778,7 +37777,7 @@
       <c r="DN111" s="83"/>
       <c r="DO111" s="84"/>
     </row>
-    <row r="112" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A112" s="164"/>
       <c r="B112" s="16" t="s">
         <v>56</v>
@@ -37907,7 +37906,7 @@
       <c r="DN112" s="83"/>
       <c r="DO112" s="84"/>
     </row>
-    <row r="113" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A113" s="164"/>
       <c r="B113" s="16" t="s">
         <v>56</v>
@@ -38036,8 +38035,8 @@
       <c r="DN113" s="83"/>
       <c r="DO113" s="84"/>
     </row>
-    <row r="114" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A114" s="165"/>
+    <row r="114" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="167"/>
       <c r="B114" s="50" t="s">
         <v>56</v>
       </c>
@@ -38165,8 +38164,8 @@
       <c r="DN114" s="83"/>
       <c r="DO114" s="84"/>
     </row>
-    <row r="115" spans="1:119" ht="55" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="166" t="s">
+    <row r="115" spans="1:119" ht="54.4" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="163" t="s">
         <v>178</v>
       </c>
       <c r="B115" s="15" t="s">
@@ -38296,7 +38295,7 @@
       <c r="DN115" s="83"/>
       <c r="DO115" s="84"/>
     </row>
-    <row r="116" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A116" s="164"/>
       <c r="B116" s="16" t="s">
         <v>56</v>
@@ -38425,7 +38424,7 @@
       <c r="DN116" s="83"/>
       <c r="DO116" s="84"/>
     </row>
-    <row r="117" spans="1:119" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:119" ht="54" x14ac:dyDescent="0.35">
       <c r="A117" s="164"/>
       <c r="B117" s="16" t="s">
         <v>56</v>
@@ -38554,7 +38553,7 @@
       <c r="DN117" s="83"/>
       <c r="DO117" s="84"/>
     </row>
-    <row r="118" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A118" s="164"/>
       <c r="B118" s="16" t="s">
         <v>56</v>
@@ -38683,7 +38682,7 @@
       <c r="DN118" s="83"/>
       <c r="DO118" s="84"/>
     </row>
-    <row r="119" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A119" s="164"/>
       <c r="B119" s="16" t="s">
         <v>56</v>
@@ -38812,7 +38811,7 @@
       <c r="DN119" s="83"/>
       <c r="DO119" s="84"/>
     </row>
-    <row r="120" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A120" s="164"/>
       <c r="B120" s="16" t="s">
         <v>56</v>
@@ -38941,7 +38940,7 @@
       <c r="DN120" s="83"/>
       <c r="DO120" s="84"/>
     </row>
-    <row r="121" spans="1:119" ht="41" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:119" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A121" s="164"/>
       <c r="B121" s="16" t="s">
         <v>56</v>
@@ -39070,8 +39069,8 @@
       <c r="DN121" s="83"/>
       <c r="DO121" s="84"/>
     </row>
-    <row r="122" spans="1:119" ht="41.35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A122" s="167"/>
+    <row r="122" spans="1:119" ht="40.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="165"/>
       <c r="B122" s="17" t="s">
         <v>56</v>
       </c>
@@ -39201,15 +39200,19 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="BT4:BU4"/>
-    <mergeCell ref="BV4:BY4"/>
-    <mergeCell ref="BZ4:CC4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:Y4"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AH4:AM4"/>
-    <mergeCell ref="AN4:AW4"/>
+    <mergeCell ref="A107:A114"/>
+    <mergeCell ref="A115:A122"/>
+    <mergeCell ref="A81:A84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A89:A92"/>
+    <mergeCell ref="A93:A96"/>
+    <mergeCell ref="A97:A106"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="A53:A62"/>
+    <mergeCell ref="A63:A72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A75:A76"/>
     <mergeCell ref="A77:A80"/>
     <mergeCell ref="DH4:DO4"/>
     <mergeCell ref="A10:A11"/>
@@ -39226,19 +39229,15 @@
     <mergeCell ref="AX4:BG4"/>
     <mergeCell ref="BH4:BQ4"/>
     <mergeCell ref="BR4:BS4"/>
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="A53:A62"/>
-    <mergeCell ref="A63:A72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A107:A114"/>
-    <mergeCell ref="A115:A122"/>
-    <mergeCell ref="A81:A84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A89:A92"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="A97:A106"/>
+    <mergeCell ref="BT4:BU4"/>
+    <mergeCell ref="BV4:BY4"/>
+    <mergeCell ref="BZ4:CC4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:Y4"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AH4:AM4"/>
+    <mergeCell ref="AN4:AW4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>